<commit_message>
Atualizado IM (separação do IM_1 em vários submapas).
</commit_message>
<xml_diff>
--- a/outputs/sisaprophelper#autoaprop/autoapropxlsx/IM_1.XLSX
+++ b/outputs/sisaprophelper#autoaprop/autoapropxlsx/IM_1.XLSX
@@ -133,13 +133,13 @@
     <t>ALDO GARCIA DA SILVA</t>
   </si>
   <si>
-    <t>MARIANA COUTINHO PONTES</t>
+    <t> </t>
   </si>
   <si>
-    <t>DAVI FELIPE PONTEL</t>
+    <t> </t>
   </si>
   <si>
-    <t>LILIAN LEITE O BRILHANTE</t>
+    <t> </t>
   </si>
   <si>
     <t> </t>
@@ -151,13 +151,13 @@
     <t>1660</t>
   </si>
   <si>
-    <t>3193</t>
+    <t> </t>
   </si>
   <si>
-    <t>3442</t>
+    <t> </t>
   </si>
   <si>
-    <t>3489</t>
+    <t> </t>
   </si>
   <si>
     <t> </t>
@@ -3523,15 +3523,15 @@
       <c r="N12" s="161"/>
       <c r="O12" s="187" t="str">
         <f>H12</f>
-        <v>MARIANA COUTINHO PONTES</v>
+        <v> </v>
       </c>
       <c r="P12" s="161" t="str">
         <f>I12</f>
-        <v>DAVI FELIPE PONTEL</v>
+        <v> </v>
       </c>
       <c r="Q12" s="161" t="str">
         <f>J12</f>
-        <v>LILIAN LEITE O BRILHANTE</v>
+        <v> </v>
       </c>
       <c r="R12" s="161" t="str">
         <f>K12</f>
@@ -3550,15 +3550,15 @@
       <c r="W12" s="161"/>
       <c r="X12" s="161" t="str">
         <f>H12</f>
-        <v>MARIANA COUTINHO PONTES</v>
+        <v> </v>
       </c>
       <c r="Y12" s="161" t="str">
         <f>I12</f>
-        <v>DAVI FELIPE PONTEL</v>
+        <v> </v>
       </c>
       <c r="Z12" s="161" t="str">
         <f>J12</f>
-        <v>LILIAN LEITE O BRILHANTE</v>
+        <v> </v>
       </c>
       <c r="AA12" s="161" t="str">
         <f>K12</f>
@@ -3574,15 +3574,15 @@
       </c>
       <c r="AD12" s="183" t="str">
         <f t="shared" si="0"/>
-        <v>MARIANA COUTINHO PONTES</v>
+        <v> </v>
       </c>
       <c r="AE12" s="161" t="str">
         <f t="shared" si="0"/>
-        <v>DAVI FELIPE PONTEL</v>
+        <v> </v>
       </c>
       <c r="AF12" s="161" t="str">
         <f t="shared" si="0"/>
-        <v>LILIAN LEITE O BRILHANTE</v>
+        <v> </v>
       </c>
       <c r="AG12" s="161" t="str">
         <f t="shared" si="0"/>
@@ -3598,15 +3598,15 @@
       </c>
       <c r="AJ12" s="183" t="str">
         <f t="shared" si="1"/>
-        <v>MARIANA COUTINHO PONTES</v>
+        <v> </v>
       </c>
       <c r="AK12" s="161" t="str">
         <f t="shared" si="1"/>
-        <v>DAVI FELIPE PONTEL</v>
+        <v> </v>
       </c>
       <c r="AL12" s="161" t="str">
         <f t="shared" si="1"/>
-        <v>LILIAN LEITE O BRILHANTE</v>
+        <v> </v>
       </c>
       <c r="AM12" s="161" t="str">
         <f t="shared" si="1"/>
@@ -3903,15 +3903,15 @@
       <c r="N19" s="172"/>
       <c r="O19" s="172" t="str">
         <f>H19</f>
-        <v>3193</v>
+        <v> </v>
       </c>
       <c r="P19" s="172" t="str">
         <f>I19</f>
-        <v>3442</v>
+        <v> </v>
       </c>
       <c r="Q19" s="172" t="str">
         <f>J19</f>
-        <v>3489</v>
+        <v> </v>
       </c>
       <c r="R19" s="172" t="str">
         <f>K19</f>
@@ -3930,15 +3930,15 @@
       <c r="W19" s="172"/>
       <c r="X19" s="172" t="str">
         <f>H19</f>
-        <v>3193</v>
+        <v> </v>
       </c>
       <c r="Y19" s="172" t="str">
         <f>I19</f>
-        <v>3442</v>
+        <v> </v>
       </c>
       <c r="Z19" s="172" t="str">
         <f>J19</f>
-        <v>3489</v>
+        <v> </v>
       </c>
       <c r="AA19" s="172" t="str">
         <f>K19</f>
@@ -3954,15 +3954,15 @@
       </c>
       <c r="AD19" s="172" t="str">
         <f t="shared" si="2"/>
-        <v>3193</v>
+        <v> </v>
       </c>
       <c r="AE19" s="172" t="str">
         <f t="shared" si="2"/>
-        <v>3442</v>
+        <v> </v>
       </c>
       <c r="AF19" s="172" t="str">
         <f t="shared" si="2"/>
-        <v>3489</v>
+        <v> </v>
       </c>
       <c r="AG19" s="172" t="str">
         <f t="shared" si="2"/>
@@ -3978,15 +3978,15 @@
       </c>
       <c r="AJ19" s="172" t="str">
         <f t="shared" si="3"/>
-        <v>3193</v>
+        <v> </v>
       </c>
       <c r="AK19" s="172" t="str">
         <f t="shared" si="3"/>
-        <v>3442</v>
+        <v> </v>
       </c>
       <c r="AL19" s="172" t="str">
         <f t="shared" si="3"/>
-        <v>3489</v>
+        <v> </v>
       </c>
       <c r="AM19" s="172" t="str">
         <f t="shared" si="3"/>
@@ -6607,15 +6607,15 @@
       </c>
       <c r="H12" s="161" t="str">
         <f>'Segunda a Sexta'!H12:H18</f>
-        <v>MARIANA COUTINHO PONTES</v>
+        <v> </v>
       </c>
       <c r="I12" s="161" t="str">
         <f>'Segunda a Sexta'!I12:I18</f>
-        <v>DAVI FELIPE PONTEL</v>
+        <v> </v>
       </c>
       <c r="J12" s="161" t="str">
         <f>'Segunda a Sexta'!J12:J18</f>
-        <v>LILIAN LEITE O BRILHANTE</v>
+        <v> </v>
       </c>
       <c r="K12" s="161" t="str">
         <f>'Segunda a Sexta'!K12:K18</f>
@@ -6632,15 +6632,15 @@
       <c r="N12" s="161"/>
       <c r="O12" s="187" t="str">
         <f>'Segunda a Sexta'!H12:H18</f>
-        <v>MARIANA COUTINHO PONTES</v>
+        <v> </v>
       </c>
       <c r="P12" s="187" t="str">
         <f>'Segunda a Sexta'!I12:I18</f>
-        <v>DAVI FELIPE PONTEL</v>
+        <v> </v>
       </c>
       <c r="Q12" s="187" t="str">
         <f>'Segunda a Sexta'!J12:J18</f>
-        <v>LILIAN LEITE O BRILHANTE</v>
+        <v> </v>
       </c>
       <c r="R12" s="187" t="str">
         <f>'Segunda a Sexta'!K12:K18</f>
@@ -6939,15 +6939,15 @@
       </c>
       <c r="H19" s="168" t="str">
         <f>'Segunda a Sexta'!H19:H20</f>
-        <v>3193</v>
+        <v> </v>
       </c>
       <c r="I19" s="168" t="str">
         <f>'Segunda a Sexta'!I19:I20</f>
-        <v>3442</v>
+        <v> </v>
       </c>
       <c r="J19" s="170" t="str">
         <f>'Segunda a Sexta'!J19:J20</f>
-        <v>3489</v>
+        <v> </v>
       </c>
       <c r="K19" s="172" t="str">
         <f>'Segunda a Sexta'!K19:K20</f>
@@ -6964,15 +6964,15 @@
       <c r="N19" s="172"/>
       <c r="O19" s="257" t="str">
         <f>'Segunda a Sexta'!H19:H20</f>
-        <v>3193</v>
+        <v> </v>
       </c>
       <c r="P19" s="257" t="str">
         <f>'Segunda a Sexta'!I19:I20</f>
-        <v>3442</v>
+        <v> </v>
       </c>
       <c r="Q19" s="257" t="str">
         <f>'Segunda a Sexta'!J19:J20</f>
-        <v>3489</v>
+        <v> </v>
       </c>
       <c r="R19" s="257" t="str">
         <f>'Segunda a Sexta'!K19:K20</f>

</xml_diff>